<commit_message>
Start to use openpyxl to fill in increased id number for each sheet
</commit_message>
<xml_diff>
--- a/dist/模板/集体资产股权确认登记表.xlsx
+++ b/dist/模板/集体资产股权确认登记表.xlsx
@@ -5,10 +5,10 @@
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sc\Desktop\others\定安县新竹镇\模板\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sc\PycharmProjects\AutoSummary\模板\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE9E5226-AD37-4D77-AA45-B8380B617CA7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA4FADC2-60EB-46FB-B224-9625BEA9F8B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
   </sheets>
   <definedNames>
     <definedName name="MmExcelLinker_5B53D910_5278_4053_934D_8868A76962F4">Sheet1!$L$10:$L$10</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$J$249</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$I$249</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Sheet1!$2:$5</definedName>
   </definedNames>
   <calcPr calcId="191029" calcOnSave="0"/>
@@ -291,6 +291,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -313,9 +316,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -595,8 +595,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J249"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A240" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="A250" sqref="A250:XFD250"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="27.6" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -614,27 +614,27 @@
   <sheetData>
     <row r="1" spans="1:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
     </row>
     <row r="3" spans="1:10" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
       <c r="G3" s="4" t="s">
         <v>10</v>
       </c>
@@ -642,44 +642,44 @@
       <c r="I3" s="2"/>
     </row>
     <row r="4" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="15" t="s">
+      <c r="D4" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="15" t="s">
+      <c r="E4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="13" t="s">
+      <c r="G4" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="10" t="s">
+      <c r="H4" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="15" t="s">
+      <c r="I4" s="7" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="15"/>
-      <c r="B5" s="15"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="15"/>
+      <c r="A5" s="7"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="7"/>
     </row>
     <row r="6" spans="1:10" ht="16.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
@@ -2973,21 +2973,21 @@
     <row r="249" ht="16.05" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
     <mergeCell ref="A3:F3"/>
     <mergeCell ref="F4:F5"/>
     <mergeCell ref="H4:H5"/>
     <mergeCell ref="A2:I2"/>
     <mergeCell ref="G4:G5"/>
     <mergeCell ref="I4:I5"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.74803149606299213" right="0.23622047244094491" top="0.98425196850393704" bottom="0.98425196850393704" header="0.51181102362204722" footer="0.51181102362204722"/>
-  <pageSetup paperSize="9" scale="73" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="82" orientation="portrait" r:id="rId1"/>
   <rowBreaks count="3" manualBreakCount="3">
     <brk id="53" max="16383" man="1"/>
     <brk id="99" max="16383" man="1"/>

</xml_diff>